<commit_message>
veränderte Ordnerstruktur und nächste Oberfläche für Kalender einträge
</commit_message>
<xml_diff>
--- a/Userstory.xlsx
+++ b/Userstory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>registration seite erstellen</t>
   </si>
@@ -123,9 +123,6 @@
     <t>email muss verifiziert werden per email senden an email</t>
   </si>
   <si>
-    <t>bis zu den Ferien im Februar</t>
-  </si>
-  <si>
     <t>geplante Zeit</t>
   </si>
   <si>
@@ -172,6 +169,27 @@
   </si>
   <si>
     <t xml:space="preserve"> - oberfläche erstellen</t>
+  </si>
+  <si>
+    <t>email schicken um account zu aktivieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - unbestätigt Status (speichern der Daten sofort, aber aktiviert Account erst wenn email bestätigt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - tokken generieren um email zu verifizieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - eine Email versenden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - gültigkeit des Tokkens muss vergehen!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - wenn sich jemand ein zweites mal mit der selben email registrieren möchte dann wird ihm eine Fehlermeldung gegeben ( keine Weiterleitung)</t>
+  </si>
+  <si>
+    <t>bis Fasching</t>
   </si>
 </sst>
 </file>
@@ -256,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -336,6 +354,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -343,7 +374,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -365,17 +396,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
@@ -659,16 +695,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="74.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -681,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,289 +728,339 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="26"/>
+        <v>42</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="25"/>
+        <v>41</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="25"/>
+        <v>45</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="25"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="26"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="25"/>
+        <v>43</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="23"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="6" t="s">
+      <c r="C21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="C22" s="27"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="6" t="s">
+      <c r="C23" s="27"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="22"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B33" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="C33" s="27"/>
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B34" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="C34" s="27"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C36" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C21:C28"/>
-    <mergeCell ref="C2:C13"/>
-    <mergeCell ref="C15:C19"/>
+  <mergeCells count="4">
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="C11:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>